<commit_message>
update notification for orderplacing
</commit_message>
<xml_diff>
--- a/Week 7/ProductBacklog (Version 0.5).xlsx
+++ b/Week 7/ProductBacklog (Version 0.5).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JavaWeb\swp391-onlineshop-gr1\Week 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\SWP\swp391-onlineshop-gr1\Week 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58177AB-7E0B-4146-A652-E1164FF10D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20595" windowHeight="7740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -280,13 +281,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -622,143 +630,143 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="26" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="27" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1114,11 +1122,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1306,8 +1314,8 @@
       <c r="G11" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>75</v>
+      <c r="H11" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="I11" s="15"/>
     </row>
@@ -1360,8 +1368,8 @@
       <c r="G13" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="18" t="s">
-        <v>75</v>
+      <c r="H13" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="I13" s="15"/>
     </row>
@@ -1495,8 +1503,8 @@
       <c r="G18" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>75</v>
+      <c r="H18" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="I18" s="15"/>
     </row>
@@ -1846,8 +1854,8 @@
       <c r="G31" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>75</v>
+      <c r="H31" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="I31" s="15"/>
     </row>

</xml_diff>